<commit_message>
Update Cloud Labs Login Credentials - Dynatrace - 28Jul-01Aug 2025 - BOA.xlsx
</commit_message>
<xml_diff>
--- a/Cloud Labs Login Credentials - Dynatrace - 28Jul-01Aug 2025 - BOA.xlsx
+++ b/Cloud Labs Login Credentials - Dynatrace - 28Jul-01Aug 2025 - BOA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\DT_BOA_28_07_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833379C6-911D-4D86-BAC9-97B56A905BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953014EE-76C1-4679-8B1D-1361CC998691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,9 +237,6 @@
     <t>IP Address</t>
   </si>
   <si>
-    <t>ec2-user</t>
-  </si>
-  <si>
     <t>107.21.63.95</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t xml:space="preserve">75.101.170.109 </t>
+  </si>
+  <si>
+    <t>ubuntu</t>
   </si>
 </sst>
 </file>
@@ -981,6 +981,8 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1011,8 +1013,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1114,9 +1114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1316355</xdr:colOff>
+      <xdr:colOff>1312545</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>440055</xdr:rowOff>
+      <xdr:rowOff>436245</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1461,7 +1461,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F7" sqref="F7:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1479,52 +1479,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
@@ -1539,10 +1539,10 @@
       <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1560,11 +1560,11 @@
         <v>3</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>94</v>
+      <c r="F7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1580,11 +1580,11 @@
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>67</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1600,11 +1600,11 @@
       <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>69</v>
+      <c r="F9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1621,11 +1621,11 @@
         <v>3</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>70</v>
+      <c r="F10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1641,11 +1641,11 @@
       <c r="D11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>71</v>
+      <c r="F11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1661,11 +1661,11 @@
       <c r="D12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>72</v>
+      <c r="F12" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1681,11 +1681,11 @@
       <c r="D13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>73</v>
+      <c r="F13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1701,11 +1701,11 @@
       <c r="D14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>74</v>
+      <c r="F14" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1721,11 +1721,11 @@
       <c r="D15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>75</v>
+      <c r="F15" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1741,11 +1741,11 @@
       <c r="D16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>76</v>
+      <c r="F16" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1761,11 +1761,11 @@
       <c r="D17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>77</v>
+      <c r="F17" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1781,11 +1781,11 @@
       <c r="D18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>78</v>
+      <c r="F18" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1801,11 +1801,11 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>79</v>
+      <c r="F19" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1821,11 +1821,11 @@
       <c r="D20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>80</v>
+      <c r="F20" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1841,11 +1841,11 @@
       <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>81</v>
+      <c r="F21" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1861,11 +1861,11 @@
       <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>82</v>
+      <c r="F22" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1881,11 +1881,11 @@
       <c r="D23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>83</v>
+      <c r="F23" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1901,11 +1901,11 @@
       <c r="D24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="26" t="s">
-        <v>84</v>
+      <c r="F24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1921,11 +1921,11 @@
       <c r="D25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>85</v>
+      <c r="F25" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1941,11 +1941,11 @@
       <c r="D26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>86</v>
+      <c r="F26" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1961,11 +1961,11 @@
       <c r="D27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>87</v>
+      <c r="F27" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -1981,11 +1981,11 @@
       <c r="D28" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>88</v>
+      <c r="F28" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -2001,11 +2001,11 @@
       <c r="D29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="26" t="s">
-        <v>89</v>
+      <c r="F29" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -2021,11 +2021,11 @@
       <c r="D30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>90</v>
+      <c r="F30" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
@@ -2041,11 +2041,11 @@
       <c r="D31" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>91</v>
+      <c r="F31" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
@@ -2061,16 +2061,16 @@
       <c r="D32" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>92</v>
+      <c r="F32" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.45">
       <c r="I33" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>